<commit_message>
Completed testing for Service
- Set up a proper testing scene for Serving
- Cleaned up PlayerStates.ServeState for serving only when interacted
- Refactored items from Player to Athlete that AI players should be able to use
- Fixed Ball change of possession
- Added change to MatchStates.InPlayState
</commit_message>
<xml_diff>
--- a/Resources/Serve Height and Distance.xlsx
+++ b/Resources/Serve Height and Distance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aaron\Documents\Unity\Projects\unity-kings-of-the-beach\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A695E9F-E346-4781-8118-DC88AE1DC3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B1A236-999D-46AB-B2F1-3BD212557067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="1" xr2:uid="{2C8E0966-E277-4FCE-B0D3-DC5E73B5EF92}"/>
+    <workbookView xWindow="18763" yWindow="797" windowWidth="12951" windowHeight="16372" activeTab="1" xr2:uid="{2C8E0966-E277-4FCE-B0D3-DC5E73B5EF92}"/>
   </bookViews>
   <sheets>
     <sheet name="Max-Min" sheetId="1" r:id="rId1"/>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E1D9BD6-3CBA-43EB-8C04-71D5EF2734A2}">
   <dimension ref="A16:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1455,14 +1455,14 @@
         <v>5</v>
       </c>
       <c r="E17" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F17" s="1">
         <v>18</v>
       </c>
       <c r="G17" s="2">
         <f>E17+(F17-E17)*(1-((A17-B17)/(D17-C17))^2)</f>
-        <v>16.555555555555557</v>
+        <v>16.777777777777779</v>
       </c>
       <c r="H17" s="2"/>
     </row>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="E18">
         <f>E17</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F18">
         <f>F17</f>
@@ -1493,7 +1493,7 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" ref="G18:G47" si="0">E18+(F18-E18)*(1-((A18-B18)/(D18-C18))^2)</f>
-        <v>16.829999999999998</v>
+        <v>17.009999999999998</v>
       </c>
       <c r="H18" s="2"/>
     </row>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
@@ -1524,7 +1524,7 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="0"/>
-        <v>17.075555555555553</v>
+        <v>17.217777777777776</v>
       </c>
       <c r="H19" s="2"/>
     </row>
@@ -1547,7 +1547,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
@@ -1555,7 +1555,7 @@
       </c>
       <c r="G20" s="2">
         <f t="shared" si="0"/>
-        <v>17.292222222222222</v>
+        <v>17.401111111111113</v>
       </c>
       <c r="H20" s="2"/>
     </row>
@@ -1578,7 +1578,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="G21" s="2">
         <f t="shared" si="0"/>
-        <v>17.48</v>
+        <v>17.560000000000002</v>
       </c>
       <c r="H21" s="2"/>
     </row>
@@ -1609,7 +1609,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
@@ -1617,7 +1617,7 @@
       </c>
       <c r="G22" s="2">
         <f t="shared" si="0"/>
-        <v>17.638888888888889</v>
+        <v>17.694444444444446</v>
       </c>
       <c r="H22" s="2"/>
     </row>
@@ -1640,7 +1640,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
@@ -1648,7 +1648,7 @@
       </c>
       <c r="G23" s="2">
         <f t="shared" si="0"/>
-        <v>17.768888888888888</v>
+        <v>17.804444444444442</v>
       </c>
       <c r="H23" s="2"/>
     </row>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
@@ -1679,7 +1679,7 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="0"/>
-        <v>17.869999999999997</v>
+        <v>17.89</v>
       </c>
       <c r="H24" s="2"/>
     </row>
@@ -1702,7 +1702,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
@@ -1710,7 +1710,7 @@
       </c>
       <c r="G25" s="2">
         <f t="shared" si="0"/>
-        <v>17.942222222222224</v>
+        <v>17.951111111111111</v>
       </c>
       <c r="H25" s="2"/>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="G26" s="2">
         <f t="shared" si="0"/>
-        <v>17.985555555555557</v>
+        <v>17.987777777777779</v>
       </c>
       <c r="H26" s="2"/>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F27">
         <f t="shared" si="2"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
@@ -1803,7 +1803,7 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="0"/>
-        <v>17.985555555555557</v>
+        <v>17.987777777777779</v>
       </c>
       <c r="H28" s="2"/>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="G29" s="2">
         <f t="shared" si="0"/>
-        <v>17.94222222222222</v>
+        <v>17.951111111111111</v>
       </c>
       <c r="H29" s="2"/>
     </row>
@@ -1857,7 +1857,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
@@ -1865,7 +1865,7 @@
       </c>
       <c r="G30" s="2">
         <f t="shared" si="0"/>
-        <v>17.869999999999997</v>
+        <v>17.89</v>
       </c>
       <c r="H30" s="2"/>
     </row>
@@ -1888,7 +1888,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="G31" s="2">
         <f t="shared" si="0"/>
-        <v>17.768888888888888</v>
+        <v>17.804444444444442</v>
       </c>
       <c r="H31" s="2"/>
     </row>
@@ -1919,7 +1919,7 @@
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="0"/>
-        <v>17.638888888888886</v>
+        <v>17.694444444444443</v>
       </c>
       <c r="H32" s="2"/>
     </row>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
@@ -1958,7 +1958,7 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="0"/>
-        <v>17.479999999999997</v>
+        <v>17.559999999999999</v>
       </c>
       <c r="H33" s="2"/>
     </row>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
@@ -1989,7 +1989,7 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="0"/>
-        <v>17.292222222222222</v>
+        <v>17.40111111111111</v>
       </c>
       <c r="H34" s="2"/>
     </row>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="E35">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F35">
         <f t="shared" si="3"/>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="G35" s="2">
         <f t="shared" si="0"/>
-        <v>17.075555555555553</v>
+        <v>17.217777777777776</v>
       </c>
       <c r="H35" s="2"/>
     </row>
@@ -2043,7 +2043,7 @@
       </c>
       <c r="E36">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F36">
         <f t="shared" si="3"/>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="G36" s="2">
         <f t="shared" si="0"/>
-        <v>16.829999999999998</v>
+        <v>17.009999999999998</v>
       </c>
       <c r="H36" s="2"/>
     </row>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F37">
         <f t="shared" si="3"/>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="G37" s="2">
         <f t="shared" si="0"/>
-        <v>16.55555555555555</v>
+        <v>16.777777777777771</v>
       </c>
       <c r="H37" s="2"/>
     </row>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="E38">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F38">
         <f t="shared" si="3"/>
@@ -2113,7 +2113,7 @@
       </c>
       <c r="G38" s="2">
         <f t="shared" si="0"/>
-        <v>16.252222222222215</v>
+        <v>16.521111111111107</v>
       </c>
       <c r="H38" s="2"/>
     </row>
@@ -2136,7 +2136,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F39">
         <f t="shared" si="3"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="G39" s="2">
         <f t="shared" si="0"/>
-        <v>15.919999999999996</v>
+        <v>16.239999999999995</v>
       </c>
       <c r="H39" s="2"/>
     </row>
@@ -2167,7 +2167,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F40">
         <f t="shared" si="3"/>
@@ -2175,7 +2175,7 @@
       </c>
       <c r="G40" s="2">
         <f t="shared" si="0"/>
-        <v>15.558888888888886</v>
+        <v>15.934444444444441</v>
       </c>
       <c r="H40" s="2"/>
     </row>
@@ -2198,7 +2198,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F41">
         <f t="shared" si="3"/>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="G41" s="2">
         <f t="shared" si="0"/>
-        <v>15.168888888888889</v>
+        <v>15.604444444444443</v>
       </c>
       <c r="H41" s="2"/>
     </row>
@@ -2229,7 +2229,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F42">
         <f t="shared" si="3"/>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="G42" s="2">
         <f t="shared" si="0"/>
-        <v>14.75</v>
+        <v>15.25</v>
       </c>
       <c r="H42" s="2"/>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F43">
         <f t="shared" si="3"/>
@@ -2268,7 +2268,7 @@
       </c>
       <c r="G43" s="2">
         <f t="shared" si="0"/>
-        <v>14.302222222222225</v>
+        <v>14.871111111111112</v>
       </c>
       <c r="H43" s="2"/>
     </row>
@@ -2291,7 +2291,7 @@
       </c>
       <c r="E44">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F44">
         <f t="shared" si="3"/>
@@ -2299,7 +2299,7 @@
       </c>
       <c r="G44" s="2">
         <f t="shared" si="0"/>
-        <v>13.825555555555558</v>
+        <v>14.46777777777778</v>
       </c>
       <c r="H44" s="2"/>
     </row>
@@ -2322,7 +2322,7 @@
       </c>
       <c r="E45">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F45">
         <f t="shared" si="3"/>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="G45" s="2">
         <f t="shared" si="0"/>
-        <v>13.320000000000004</v>
+        <v>14.040000000000003</v>
       </c>
       <c r="H45" s="2"/>
     </row>
@@ -2353,7 +2353,7 @@
       </c>
       <c r="E46">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F46">
         <f t="shared" si="3"/>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="G46" s="2">
         <f t="shared" si="0"/>
-        <v>12.785555555555563</v>
+        <v>13.587777777777784</v>
       </c>
       <c r="H46" s="2"/>
     </row>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="E47">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F47">
         <f t="shared" si="3"/>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="G47" s="2">
         <f t="shared" si="0"/>
-        <v>12.222222222222232</v>
+        <v>13.11111111111112</v>
       </c>
       <c r="H47" s="2"/>
     </row>

</xml_diff>